<commit_message>
Disable carbon border adjustments and carbon tax on agricultural and water and waste process emissions in BAU, update WebAppData text to reflect changes
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/BDCTBA/Boolean Disable Carbon Tax Border Adjustment.xlsx
+++ b/InputData/ctrl-settings/BDCTBA/Boolean Disable Carbon Tax Border Adjustment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\ctrl-settings\BDCTBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0A652D-3E15-4320-A2BE-3B11CD7652AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E7D65B-1630-457E-83C3-A8F9AD7513A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7845" yWindow="2985" windowWidth="21600" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -44,13 +44,13 @@
     <t>As a boolean lever, use "1" to disable the carbon tax border adjustment.</t>
   </si>
   <si>
-    <t>By default, the EPS assumes carbon tax border adjustments apply across</t>
-  </si>
-  <si>
     <t>industries.</t>
   </si>
   <si>
     <t>Diable Carbon Tax Border Adjustment</t>
+  </si>
+  <si>
+    <t>By default, the EPS assumes carbon tax border adjustments do not apply across</t>
   </si>
 </sst>
 </file>
@@ -438,49 +438,49 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -497,22 +497,22 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>